<commit_message>
fixed the invoice report issue and added the new feature for the invoice report
</commit_message>
<xml_diff>
--- a/mat-backend/invoiceReports.xlsx
+++ b/mat-backend/invoiceReports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="156">
   <si>
     <t>Sl No</t>
   </si>
@@ -58,424 +58,430 @@
     <t>Total</t>
   </si>
   <si>
-    <t>IAMPL, Hosur</t>
-  </si>
-  <si>
-    <t>Station Commander 37 Wing, AFS</t>
-  </si>
-  <si>
-    <t>HAL-BKP Division</t>
-  </si>
-  <si>
-    <t>Lakshmi Machine Works Ltd</t>
-  </si>
-  <si>
-    <t>RCI/Program AD-DRDO, Hyderabad</t>
+    <t>Pushpak Industrial Services</t>
+  </si>
+  <si>
+    <t>International Aerospace Manufacturing Pvt.Ltd.,</t>
+  </si>
+  <si>
+    <t>Tata Sikorsky Aerospace Ltd</t>
+  </si>
+  <si>
+    <t>OM AGENCIES</t>
+  </si>
+  <si>
+    <t>Zoku Design and Technologies Pvt. Ltd</t>
+  </si>
+  <si>
+    <t>Zishta Traditional Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Kanchan Enterprises</t>
   </si>
   <si>
     <t>Revati Matals Crafts</t>
   </si>
   <si>
-    <t>SEC Industries Pvt ltd</t>
-  </si>
-  <si>
-    <t>IAMPL, Bangalore</t>
-  </si>
-  <si>
-    <t>Studio Coppre Pvt Ltd</t>
-  </si>
-  <si>
-    <t>Godrej &amp; Boyce Mfg.Co.Ltd</t>
-  </si>
-  <si>
-    <t>AOC 29 ED, AFS Kanpur</t>
-  </si>
-  <si>
-    <t>National Aerospace Laboratories, Banglore</t>
+    <t>HINDUSTAN AERONAUTICS LIMITED</t>
+  </si>
+  <si>
+    <t>Test Customer</t>
+  </si>
+  <si>
+    <t>The Director, National Aerospace Laboratories, Banglore</t>
+  </si>
+  <si>
+    <t>29AGCPP0679G1Z5</t>
+  </si>
+  <si>
+    <t>29AACCI4063N1Z6</t>
+  </si>
+  <si>
+    <t>36AAMCS1225J1Z9</t>
+  </si>
+  <si>
+    <t>09AEIPR1961B1ZI</t>
   </si>
   <si>
     <t>33AACCI4063N1ZH</t>
   </si>
   <si>
-    <t>35AAAGS0499C2ZB</t>
-  </si>
-  <si>
-    <t>29AAACH3641R1Z3</t>
-  </si>
-  <si>
-    <t>33AAACL5244N1ZF</t>
-  </si>
-  <si>
-    <t>Not Available</t>
+    <t>33AAACZ8718M2ZT</t>
+  </si>
+  <si>
+    <t>29AACCZ0706D1ZK</t>
+  </si>
+  <si>
+    <t>29AGRPJ7437M1ZH</t>
   </si>
   <si>
     <t>27ABGPK1717P1ZC</t>
   </si>
   <si>
-    <t>36AADCS4199N1ZN</t>
-  </si>
-  <si>
-    <t>29AACCI4063N1Z6</t>
-  </si>
-  <si>
-    <t>27AAUCS6074K2KG</t>
-  </si>
-  <si>
-    <t>27AAACG1395D1ZU</t>
-  </si>
-  <si>
-    <t>09KNPI00073D1DZ</t>
+    <t>19AAACH3641R1Z4</t>
+  </si>
+  <si>
+    <t>1234567890abcde</t>
   </si>
   <si>
     <t>29AAATC2716R1ZB</t>
   </si>
   <si>
-    <t>001/2024-25</t>
-  </si>
-  <si>
-    <t>002/2024-25</t>
-  </si>
-  <si>
-    <t>003/2024-25</t>
-  </si>
-  <si>
-    <t>004/2024-25</t>
-  </si>
-  <si>
-    <t>005/2024-25</t>
-  </si>
-  <si>
-    <t>006/2024-25</t>
-  </si>
-  <si>
-    <t>007/2024-25</t>
-  </si>
-  <si>
-    <t>008/2024-25</t>
-  </si>
-  <si>
-    <t>010/2024-25</t>
-  </si>
-  <si>
-    <t>011/2024-25</t>
-  </si>
-  <si>
-    <t>012/2024-25</t>
-  </si>
-  <si>
-    <t>013/2024-25</t>
-  </si>
-  <si>
-    <t>014/2024-25</t>
-  </si>
-  <si>
-    <t>016/2024-25</t>
-  </si>
-  <si>
-    <t>018/2024-25</t>
-  </si>
-  <si>
-    <t>019/2024-25</t>
-  </si>
-  <si>
-    <t>06-08-2024</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>12-08-2024</t>
-  </si>
-  <si>
-    <t>13-08-2024</t>
-  </si>
-  <si>
-    <t>23-08-2024</t>
+    <t>027/2024-25</t>
+  </si>
+  <si>
+    <t>028/2024-25</t>
+  </si>
+  <si>
+    <t>029/2024-25</t>
+  </si>
+  <si>
+    <t>030/2024-25</t>
+  </si>
+  <si>
+    <t>031/2024-25</t>
+  </si>
+  <si>
+    <t>032/2024-25</t>
+  </si>
+  <si>
+    <t>033/2024-25</t>
+  </si>
+  <si>
+    <t>034/2024-25</t>
+  </si>
+  <si>
+    <t>035/2024-25</t>
+  </si>
+  <si>
+    <t>036/2024-25</t>
+  </si>
+  <si>
+    <t>037/2024-25</t>
+  </si>
+  <si>
+    <t>038/2024-25</t>
+  </si>
+  <si>
+    <t>039/2024-25</t>
+  </si>
+  <si>
+    <t>040/2024-25</t>
+  </si>
+  <si>
+    <t>041/2024-25</t>
+  </si>
+  <si>
+    <t>042/2024-25</t>
+  </si>
+  <si>
+    <t>043/2024-25</t>
+  </si>
+  <si>
+    <t>044/2024-25</t>
+  </si>
+  <si>
+    <t>045/2024-25</t>
+  </si>
+  <si>
+    <t>046/2024-25</t>
+  </si>
+  <si>
+    <t>047/2024-25</t>
+  </si>
+  <si>
+    <t>048/2024-25</t>
+  </si>
+  <si>
+    <t>04-09-2024</t>
+  </si>
+  <si>
+    <t>12-09-2024</t>
   </si>
   <si>
     <t>32081090</t>
   </si>
   <si>
-    <t>32089090</t>
+    <t>38140010</t>
   </si>
   <si>
     <t>34031900</t>
   </si>
   <si>
-    <t>9965</t>
-  </si>
-  <si>
-    <t>38140010</t>
-  </si>
-  <si>
-    <t>586520.00</t>
-  </si>
-  <si>
-    <t>337.32</t>
-  </si>
-  <si>
-    <t>18500.00</t>
-  </si>
-  <si>
-    <t>102200.00</t>
-  </si>
-  <si>
-    <t>36733.95</t>
-  </si>
-  <si>
-    <t>90050.00</t>
-  </si>
-  <si>
-    <t>67115.00</t>
-  </si>
-  <si>
-    <t>1340.00</t>
-  </si>
-  <si>
-    <t>44075.00</t>
-  </si>
-  <si>
-    <t>880.00</t>
+    <t>1213</t>
+  </si>
+  <si>
+    <t>8569</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>48500.00</t>
+  </si>
+  <si>
+    <t>97000.00</t>
+  </si>
+  <si>
+    <t>320400.00</t>
+  </si>
+  <si>
+    <t>380290.00</t>
+  </si>
+  <si>
+    <t>33525.00</t>
+  </si>
+  <si>
+    <t>2966.00</t>
+  </si>
+  <si>
+    <t>743750.00</t>
+  </si>
+  <si>
+    <t>1020430.00</t>
+  </si>
+  <si>
+    <t>74700.00</t>
+  </si>
+  <si>
+    <t>33070.00</t>
+  </si>
+  <si>
+    <t>890000.00</t>
+  </si>
+  <si>
+    <t>49950.00</t>
+  </si>
+  <si>
+    <t>750.00</t>
+  </si>
+  <si>
+    <t>275440.00</t>
   </si>
   <si>
     <t>24975.00</t>
   </si>
   <si>
-    <t>80875.00</t>
-  </si>
-  <si>
-    <t>34175.00</t>
-  </si>
-  <si>
-    <t>37350.00</t>
-  </si>
-  <si>
-    <t>1337230.00</t>
-  </si>
-  <si>
-    <t>49950.00</t>
-  </si>
-  <si>
-    <t>1300.00</t>
-  </si>
-  <si>
-    <t>139796.40</t>
-  </si>
-  <si>
-    <t>117450.00</t>
-  </si>
-  <si>
-    <t>106800.00</t>
-  </si>
-  <si>
-    <t>106.80</t>
+    <t>1000.00</t>
+  </si>
+  <si>
+    <t>51200.00</t>
+  </si>
+  <si>
+    <t>1068000.00</t>
+  </si>
+  <si>
+    <t>285000.00</t>
+  </si>
+  <si>
+    <t>21150.00</t>
+  </si>
+  <si>
+    <t>600.66</t>
+  </si>
+  <si>
+    <t>50.36</t>
+  </si>
+  <si>
+    <t>10.00</t>
   </si>
   <si>
     <t>68610.00</t>
   </si>
   <si>
-    <t>5.00</t>
-  </si>
-  <si>
-    <t>11325.00</t>
+    <t>600.00</t>
+  </si>
+  <si>
+    <t>2500.00</t>
+  </si>
+  <si>
+    <t>5726272.02</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>68452.20</t>
+  </si>
+  <si>
+    <t>6034.50</t>
+  </si>
+  <si>
+    <t>533.88</t>
+  </si>
+  <si>
+    <t>133875.00</t>
+  </si>
+  <si>
+    <t>8991.00</t>
+  </si>
+  <si>
+    <t>135.00</t>
+  </si>
+  <si>
+    <t>49579.20</t>
+  </si>
+  <si>
+    <t>4495.50</t>
+  </si>
+  <si>
+    <t>180.00</t>
+  </si>
+  <si>
+    <t>3807.00</t>
+  </si>
+  <si>
+    <t>108.12</t>
+  </si>
+  <si>
+    <t>9.06</t>
+  </si>
+  <si>
+    <t>1.80</t>
+  </si>
+  <si>
+    <t>108.00</t>
+  </si>
+  <si>
+    <t>450.00</t>
+  </si>
+  <si>
+    <t>276760.26</t>
+  </si>
+  <si>
+    <t>4365.00</t>
+  </si>
+  <si>
+    <t>8730.00</t>
+  </si>
+  <si>
+    <t>28836.00</t>
+  </si>
+  <si>
+    <t>91838.70</t>
+  </si>
+  <si>
+    <t>6723.00</t>
+  </si>
+  <si>
+    <t>2247.75</t>
+  </si>
+  <si>
+    <t>90.00</t>
+  </si>
+  <si>
+    <t>4608.00</t>
+  </si>
+  <si>
+    <t>96120.00</t>
+  </si>
+  <si>
+    <t>25650.00</t>
+  </si>
+  <si>
+    <t>6174.90</t>
+  </si>
+  <si>
+    <t>293908.05</t>
+  </si>
+  <si>
+    <t>57230.00</t>
+  </si>
+  <si>
+    <t>114460.00</t>
+  </si>
+  <si>
+    <t>378072.00</t>
+  </si>
+  <si>
+    <t>448742.00</t>
+  </si>
+  <si>
+    <t>39560.00</t>
+  </si>
+  <si>
+    <t>3500.00</t>
+  </si>
+  <si>
+    <t>877625.00</t>
+  </si>
+  <si>
+    <t>1204107.00</t>
+  </si>
+  <si>
+    <t>88146.00</t>
+  </si>
+  <si>
+    <t>58941.00</t>
+  </si>
+  <si>
+    <t>885.00</t>
+  </si>
+  <si>
+    <t>325019.00</t>
+  </si>
+  <si>
+    <t>29470.00</t>
+  </si>
+  <si>
+    <t>1180.00</t>
+  </si>
+  <si>
+    <t>60416.00</t>
+  </si>
+  <si>
+    <t>1260240.00</t>
+  </si>
+  <si>
+    <t>336300.00</t>
+  </si>
+  <si>
+    <t>24957.00</t>
+  </si>
+  <si>
+    <t>709.00</t>
+  </si>
+  <si>
+    <t>59.00</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>80960.00</t>
+  </si>
+  <si>
+    <t>708.00</t>
+  </si>
+  <si>
+    <t>2950.00</t>
+  </si>
+  <si>
+    <t>6590848.00</t>
+  </si>
+  <si>
+    <t>-0.20</t>
   </si>
   <si>
     <t>0.50</t>
   </si>
   <si>
-    <t>388172.00</t>
-  </si>
-  <si>
-    <t>48975.00</t>
-  </si>
-  <si>
-    <t>3512296.97</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>3330.00</t>
-  </si>
-  <si>
-    <t>18396.00</t>
-  </si>
-  <si>
-    <t>6612.11</t>
-  </si>
-  <si>
-    <t>16209.00</t>
-  </si>
-  <si>
-    <t>12080.70</t>
-  </si>
-  <si>
-    <t>241.20</t>
-  </si>
-  <si>
-    <t>7933.50</t>
-  </si>
-  <si>
-    <t>158.40</t>
-  </si>
-  <si>
-    <t>4495.50</t>
-  </si>
-  <si>
-    <t>14557.50</t>
-  </si>
-  <si>
-    <t>6151.50</t>
-  </si>
-  <si>
-    <t>8991.00</t>
-  </si>
-  <si>
-    <t>234.00</t>
-  </si>
-  <si>
-    <t>25163.35</t>
-  </si>
-  <si>
-    <t>21141.00</t>
-  </si>
-  <si>
-    <t>166835.76</t>
-  </si>
-  <si>
-    <t>3361.50</t>
-  </si>
-  <si>
-    <t>120350.70</t>
-  </si>
-  <si>
-    <t>6174.90</t>
-  </si>
-  <si>
-    <t>0.45</t>
-  </si>
-  <si>
-    <t>1019.25</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>34935.48</t>
-  </si>
-  <si>
-    <t>4407.75</t>
-  </si>
-  <si>
-    <t>170250.07</t>
-  </si>
-  <si>
-    <t>337.00</t>
-  </si>
-  <si>
-    <t>21830.00</t>
-  </si>
-  <si>
-    <t>120596.00</t>
-  </si>
-  <si>
-    <t>43346.00</t>
-  </si>
-  <si>
-    <t>106259.00</t>
-  </si>
-  <si>
-    <t>79196.00</t>
-  </si>
-  <si>
-    <t>1581.00</t>
-  </si>
-  <si>
-    <t>52008.00</t>
-  </si>
-  <si>
-    <t>1038.00</t>
-  </si>
-  <si>
-    <t>29470.00</t>
-  </si>
-  <si>
-    <t>95432.00</t>
-  </si>
-  <si>
-    <t>40326.00</t>
-  </si>
-  <si>
-    <t>44073.00</t>
-  </si>
-  <si>
-    <t>1577931.00</t>
-  </si>
-  <si>
-    <t>58941.00</t>
-  </si>
-  <si>
-    <t>1534.00</t>
-  </si>
-  <si>
-    <t>164960.00</t>
-  </si>
-  <si>
-    <t>138591.00</t>
-  </si>
-  <si>
-    <t>107.00</t>
-  </si>
-  <si>
-    <t>80960.00</t>
-  </si>
-  <si>
-    <t>6.00</t>
-  </si>
-  <si>
-    <t>13364.00</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>458043.00</t>
-  </si>
-  <si>
-    <t>57790.00</t>
-  </si>
-  <si>
-    <t>4019633.00</t>
-  </si>
-  <si>
-    <t>-0.32</t>
-  </si>
-  <si>
-    <t>-0.06</t>
-  </si>
-  <si>
-    <t>0.30</t>
-  </si>
-  <si>
-    <t>-0.20</t>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>-0.40</t>
   </si>
   <si>
     <t>-0.50</t>
   </si>
   <si>
-    <t>-0.40</t>
-  </si>
-  <si>
-    <t>0.25</t>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>-0.42</t>
   </si>
   <si>
     <t>0.20</t>
-  </si>
-  <si>
-    <t>0.10</t>
-  </si>
-  <si>
-    <t>0.42</t>
   </si>
 </sst>
 </file>
@@ -833,7 +839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -888,37 +894,37 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="K2" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="M2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -929,34 +935,37 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="K3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="L3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="M3" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -967,37 +976,37 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="L4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="M4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1005,40 +1014,40 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
         <v>61</v>
       </c>
       <c r="G5">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L5" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="M5" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1049,37 +1058,37 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L6" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="M6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1087,40 +1096,37 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" t="s">
         <v>59</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L7" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="M7" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1128,40 +1134,40 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L8" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="M8" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1169,40 +1175,40 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J9" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="L9" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="M9" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1210,40 +1216,40 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="K10" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="L10" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="M10" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1251,40 +1257,40 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L11" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="M11" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1292,40 +1298,40 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="J12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L12" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1333,40 +1339,40 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L13" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="M13" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1374,40 +1380,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L14" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="M14" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1415,40 +1418,40 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="J15" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="K15" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="L15" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="M15" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1456,40 +1459,40 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G16">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J16" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="K16" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="L16" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="M16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1497,40 +1500,37 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" t="s">
         <v>59</v>
       </c>
       <c r="G17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="K17" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="L17" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1538,37 +1538,40 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I18" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J18" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="K18" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="L18" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="M18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1576,40 +1579,40 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H19" t="s">
         <v>81</v>
       </c>
       <c r="I19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M19" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1617,34 +1620,37 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="J20" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="K20" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="L20" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="M20" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1652,40 +1658,40 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="H21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="J21" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="K21" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="L21" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="M21" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1693,40 +1699,40 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="H22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J22" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="K22" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="L22" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="M22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1734,37 +1740,40 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>63</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I23" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="J23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L23" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M23" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1772,40 +1781,40 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L24" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="M24" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1813,40 +1822,40 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G25">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I25" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="J25" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="K25" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="L25" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="M25" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1854,37 +1863,37 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G26">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="J26" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="K26" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="L26" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="M26" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1892,40 +1901,40 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H27" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J27" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K27" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="L27" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="M27" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1933,37 +1942,40 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="F28" t="s">
+        <v>61</v>
       </c>
       <c r="G28">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J28" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="K28" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="L28" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="M28" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1971,40 +1983,40 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G29">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="H29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J29" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="K29" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="L29" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="M29" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -2012,45 +2024,63 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G30">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H30" t="s">
         <v>90</v>
       </c>
       <c r="I30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J30" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="K30" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="L30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="M30" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" t="s">
-        <v>13</v>
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
       </c>
       <c r="H31" t="s">
         <v>91</v>
@@ -2059,13 +2089,74 @@
         <v>108</v>
       </c>
       <c r="J31" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="K31" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="L31" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="M31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K32" t="s">
+        <v>94</v>
+      </c>
+      <c r="L32" t="s">
+        <v>146</v>
+      </c>
+      <c r="M32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" t="s">
+        <v>110</v>
+      </c>
+      <c r="J33" t="s">
+        <v>122</v>
+      </c>
+      <c r="K33" t="s">
+        <v>122</v>
+      </c>
+      <c r="L33" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>